<commit_message>
Selenium con archivos excel v1.1
</commit_message>
<xml_diff>
--- a/HolaMundoMaven/src/main/resources/Files/actividades.xlsx
+++ b/HolaMundoMaven/src/main/resources/Files/actividades.xlsx
@@ -24,17 +24,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Daily Status - A&amp;D</t>
-  </si>
-  <si>
-    <t>¿Qué se hizo ayer?
-¿Qué voy hacer hoy?
-Impedimentos</t>
-  </si>
-  <si>
-    <t>29/09/2021</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>Entrega de actividades</t>
+  </si>
+  <si>
+    <t>Entrega de conocimientos tras salida del equipo de System Test</t>
+  </si>
+  <si>
+    <t>22/10/2021</t>
+  </si>
+  <si>
+    <t>25/10/2021</t>
+  </si>
+  <si>
+    <t>26/10/2021</t>
+  </si>
+  <si>
+    <t>27/10/2021</t>
+  </si>
+  <si>
+    <t>28/10/2021</t>
+  </si>
+  <si>
+    <t>29/10/2021</t>
   </si>
 </sst>
 </file>
@@ -70,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -79,6 +101,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -361,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,25 +397,128 @@
     <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="31.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="31.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>